<commit_message>
Trying MJCellMatrix - mostly working with MyMatrix
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>Spot</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>DP+DC = ZC</t>
+  </si>
+  <si>
+    <t>MC Price</t>
   </si>
 </sst>
 </file>
@@ -166,7 +169,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.10917722788796001"/>
+          <c:x val="0.10917722788796008"/>
           <c:y val="0"/>
         </c:manualLayout>
       </c:layout>
@@ -1536,11 +1539,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="81680256"/>
-        <c:axId val="81715584"/>
+        <c:axId val="69474944"/>
+        <c:axId val="84219008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81680256"/>
+        <c:axId val="69474944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1565,12 +1568,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81715584"/>
+        <c:crossAx val="84219008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81715584"/>
+        <c:axId val="84219008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1596,7 +1599,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81680256"/>
+        <c:crossAx val="69474944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1608,7 +1611,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1624,8 +1627,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.26891632006966243"/>
-          <c:y val="2.8275009877756621E-2"/>
+          <c:x val="0.26891632006966293"/>
+          <c:y val="2.8275009877756645E-2"/>
           <c:w val="0.6738373047041657"/>
           <c:h val="0.8971166436276885"/>
         </c:manualLayout>
@@ -2952,23 +2955,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="81864576"/>
-        <c:axId val="81866112"/>
+        <c:axId val="84249216"/>
+        <c:axId val="84259200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81864576"/>
+        <c:axId val="84249216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81866112"/>
+        <c:crossAx val="84259200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81866112"/>
+        <c:axId val="84259200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2976,7 +2979,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81864576"/>
+        <c:crossAx val="84249216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2988,7 +2991,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3026,8 +3029,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.10951222115528757"/>
-          <c:y val="6.4986002424438482E-3"/>
+          <c:x val="0.10951222115528768"/>
+          <c:y val="6.498600242443856E-3"/>
         </c:manualLayout>
       </c:layout>
     </c:title>
@@ -3039,7 +3042,7 @@
           <c:yMode val="edge"/>
           <c:x val="8.4488407699037621E-2"/>
           <c:y val="0.19461706996942271"/>
-          <c:w val="0.85871446655282746"/>
+          <c:w val="0.85871446655282813"/>
           <c:h val="0.63890604507981763"/>
         </c:manualLayout>
       </c:layout>
@@ -3380,23 +3383,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="81894016"/>
-        <c:axId val="81912192"/>
+        <c:axId val="84274560"/>
+        <c:axId val="94966912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81894016"/>
+        <c:axId val="84274560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81912192"/>
+        <c:crossAx val="94966912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81912192"/>
+        <c:axId val="94966912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3404,7 +3407,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81894016"/>
+        <c:crossAx val="84274560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3413,7 +3416,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3430,10 +3433,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.25478018372703426"/>
-          <c:y val="6.9852153885822457E-2"/>
+          <c:x val="0.25478018372703432"/>
+          <c:y val="6.9852153885822513E-2"/>
           <c:w val="0.68596981627296583"/>
-          <c:h val="0.79841818205655968"/>
+          <c:h val="0.79841818205655957"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3767,23 +3770,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="81919360"/>
-        <c:axId val="90707072"/>
+        <c:axId val="94986624"/>
+        <c:axId val="94988160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81919360"/>
+        <c:axId val="94986624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90707072"/>
+        <c:crossAx val="94988160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90707072"/>
+        <c:axId val="94988160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3791,7 +3794,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81919360"/>
+        <c:crossAx val="94986624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3803,7 +3806,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4104,11 +4107,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="90739456"/>
-        <c:axId val="90741376"/>
+        <c:axId val="95229440"/>
+        <c:axId val="95231360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="90739456"/>
+        <c:axId val="95229440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4117,12 +4120,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90741376"/>
+        <c:crossAx val="95231360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90741376"/>
+        <c:axId val="95231360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4132,7 +4135,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90739456"/>
+        <c:crossAx val="95229440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4141,7 +4144,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4587,10 +4590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S347"/>
+  <dimension ref="A1:S355"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A289" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G342" sqref="G342"/>
+    <sheetView tabSelected="1" topLeftCell="E350" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J356" sqref="J356"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15953,7 +15956,7 @@
         <v>52</v>
       </c>
       <c r="D299">
-        <f t="shared" ref="D299:D330" si="22">100+B299</f>
+        <f t="shared" ref="D299" si="22">100+B299</f>
         <v>100</v>
       </c>
       <c r="E299">
@@ -16018,7 +16021,7 @@
         <v>54</v>
       </c>
       <c r="D301">
-        <f t="shared" ref="D301:D347" si="23">100+B301</f>
+        <f t="shared" ref="D301" si="23">100+B301</f>
         <v>100</v>
       </c>
       <c r="E301">
@@ -16083,7 +16086,7 @@
         <v>56</v>
       </c>
       <c r="D303">
-        <f t="shared" ref="D303:D347" si="24">100+B303</f>
+        <f t="shared" ref="D303" si="24">100+B303</f>
         <v>100</v>
       </c>
       <c r="E303">
@@ -16148,7 +16151,7 @@
         <v>58</v>
       </c>
       <c r="D305">
-        <f t="shared" ref="D305:D347" si="25">100+B305</f>
+        <f t="shared" ref="D305" si="25">100+B305</f>
         <v>100</v>
       </c>
       <c r="E305">
@@ -16213,7 +16216,7 @@
         <v>60</v>
       </c>
       <c r="D307">
-        <f t="shared" ref="D307:D347" si="26">100+B307</f>
+        <f t="shared" ref="D307" si="26">100+B307</f>
         <v>100</v>
       </c>
       <c r="E307">
@@ -16278,7 +16281,7 @@
         <v>62</v>
       </c>
       <c r="D309">
-        <f t="shared" ref="D309:D347" si="27">100+B309</f>
+        <f t="shared" ref="D309" si="27">100+B309</f>
         <v>100</v>
       </c>
       <c r="E309">
@@ -16343,7 +16346,7 @@
         <v>64</v>
       </c>
       <c r="D311">
-        <f t="shared" ref="D311:D347" si="28">100+B311</f>
+        <f t="shared" ref="D311" si="28">100+B311</f>
         <v>100</v>
       </c>
       <c r="E311">
@@ -16408,7 +16411,7 @@
         <v>66</v>
       </c>
       <c r="D313">
-        <f t="shared" ref="D313:D347" si="29">100+B313</f>
+        <f t="shared" ref="D313" si="29">100+B313</f>
         <v>100</v>
       </c>
       <c r="E313">
@@ -16473,7 +16476,7 @@
         <v>68</v>
       </c>
       <c r="D315">
-        <f t="shared" ref="D315:D347" si="30">100+B315</f>
+        <f t="shared" ref="D315" si="30">100+B315</f>
         <v>100</v>
       </c>
       <c r="E315">
@@ -16538,7 +16541,7 @@
         <v>70</v>
       </c>
       <c r="D317">
-        <f t="shared" ref="D317:D347" si="31">100+B317</f>
+        <f t="shared" ref="D317" si="31">100+B317</f>
         <v>100</v>
       </c>
       <c r="E317">
@@ -16603,7 +16606,7 @@
         <v>72</v>
       </c>
       <c r="D319">
-        <f t="shared" ref="D319:D347" si="32">100+B319</f>
+        <f t="shared" ref="D319" si="32">100+B319</f>
         <v>100</v>
       </c>
       <c r="E319">
@@ -16668,7 +16671,7 @@
         <v>74</v>
       </c>
       <c r="D321">
-        <f t="shared" ref="D321:D347" si="33">100+B321</f>
+        <f t="shared" ref="D321" si="33">100+B321</f>
         <v>100</v>
       </c>
       <c r="E321">
@@ -16733,7 +16736,7 @@
         <v>76</v>
       </c>
       <c r="D323">
-        <f t="shared" ref="D323:D347" si="34">100+B323</f>
+        <f t="shared" ref="D323" si="34">100+B323</f>
         <v>100</v>
       </c>
       <c r="E323">
@@ -16798,7 +16801,7 @@
         <v>78</v>
       </c>
       <c r="D325">
-        <f t="shared" ref="D325:D347" si="35">100+B325</f>
+        <f t="shared" ref="D325" si="35">100+B325</f>
         <v>100</v>
       </c>
       <c r="E325">
@@ -16863,7 +16866,7 @@
         <v>80</v>
       </c>
       <c r="D327">
-        <f t="shared" ref="D327:D347" si="36">100+B327</f>
+        <f t="shared" ref="D327" si="36">100+B327</f>
         <v>100</v>
       </c>
       <c r="E327">
@@ -16928,7 +16931,7 @@
         <v>82</v>
       </c>
       <c r="D329">
-        <f t="shared" ref="D329:D347" si="37">100+B329</f>
+        <f t="shared" ref="D329" si="37">100+B329</f>
         <v>100</v>
       </c>
       <c r="E329">
@@ -16993,7 +16996,7 @@
         <v>84</v>
       </c>
       <c r="D331">
-        <f t="shared" ref="D331:D347" si="38">100+B331</f>
+        <f t="shared" ref="D331" si="38">100+B331</f>
         <v>100</v>
       </c>
       <c r="E331">
@@ -17058,7 +17061,7 @@
         <v>86</v>
       </c>
       <c r="D333">
-        <f t="shared" ref="D333:D347" si="39">100+B333</f>
+        <f t="shared" ref="D333" si="39">100+B333</f>
         <v>100</v>
       </c>
       <c r="E333">
@@ -17123,7 +17126,7 @@
         <v>88</v>
       </c>
       <c r="D335">
-        <f t="shared" ref="D335:D347" si="40">100+B335</f>
+        <f t="shared" ref="D335" si="40">100+B335</f>
         <v>100</v>
       </c>
       <c r="E335">
@@ -17188,7 +17191,7 @@
         <v>90</v>
       </c>
       <c r="D337">
-        <f t="shared" ref="D337:D347" si="41">100+B337</f>
+        <f t="shared" ref="D337" si="41">100+B337</f>
         <v>100</v>
       </c>
       <c r="E337">
@@ -17253,7 +17256,7 @@
         <v>92</v>
       </c>
       <c r="D339">
-        <f t="shared" ref="D339:D347" si="42">100+B339</f>
+        <f t="shared" ref="D339" si="42">100+B339</f>
         <v>100</v>
       </c>
       <c r="E339">
@@ -17318,7 +17321,7 @@
         <v>94</v>
       </c>
       <c r="D341">
-        <f t="shared" ref="D341:D347" si="43">100+B341</f>
+        <f t="shared" ref="D341" si="43">100+B341</f>
         <v>100</v>
       </c>
       <c r="E341">
@@ -17383,7 +17386,7 @@
         <v>96</v>
       </c>
       <c r="D343">
-        <f t="shared" ref="D343:D347" si="44">100+B343</f>
+        <f t="shared" ref="D343" si="44">100+B343</f>
         <v>100</v>
       </c>
       <c r="E343">
@@ -17448,7 +17451,7 @@
         <v>98</v>
       </c>
       <c r="D345">
-        <f t="shared" ref="D345:D347" si="45">100+B345</f>
+        <f t="shared" ref="D345" si="45">100+B345</f>
         <v>100</v>
       </c>
       <c r="E345">
@@ -17539,6 +17542,67 @@
       <c r="K347" t="b">
         <f t="shared" si="21"/>
         <v>1</v>
+      </c>
+    </row>
+    <row r="350" spans="3:11">
+      <c r="F350">
+        <v>1</v>
+      </c>
+      <c r="G350">
+        <v>1</v>
+      </c>
+      <c r="I350">
+        <v>1</v>
+      </c>
+      <c r="J350">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="351" spans="3:11">
+      <c r="F351">
+        <v>1</v>
+      </c>
+      <c r="G351">
+        <v>1</v>
+      </c>
+      <c r="I351">
+        <v>1</v>
+      </c>
+      <c r="J351">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="354" spans="3:10">
+      <c r="J354" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="355" spans="3:10">
+      <c r="C355">
+        <v>100</v>
+      </c>
+      <c r="D355">
+        <f t="shared" ref="D355" si="47">100+B355</f>
+        <v>100</v>
+      </c>
+      <c r="E355">
+        <v>0.05</v>
+      </c>
+      <c r="F355">
+        <v>0</v>
+      </c>
+      <c r="G355">
+        <v>0.15</v>
+      </c>
+      <c r="H355">
+        <v>1</v>
+      </c>
+      <c r="I355">
+        <v>1000</v>
+      </c>
+      <c r="J355">
+        <f>MCVanillaCall(C355:I355)</f>
+        <v>8.5331695996331316</v>
       </c>
     </row>
   </sheetData>

</xml_diff>